<commit_message>
almost outputted header with first selected date
</commit_message>
<xml_diff>
--- a/Findings Tracker.xlsx
+++ b/Findings Tracker.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s300102\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1551b3744a113d45/Documents/UiPath/Robotic_Process_Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_A2C0EC805502C7573C1CFB3FD43E70FF7298FEE5" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FindingsTracker" sheetId="1" r:id="rId1"/>
@@ -329,7 +330,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -689,31 +690,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H14"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="4" width="61" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
-    <col min="12" max="12" width="92.42578125" customWidth="1"/>
+    <col min="12" max="12" width="92.44140625" customWidth="1"/>
     <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="54" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,7 +755,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>43839</v>
       </c>
@@ -795,7 +796,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>43839</v>
       </c>
@@ -836,7 +837,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>43839</v>
       </c>
@@ -877,7 +878,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>43839</v>
       </c>
@@ -918,7 +919,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>43843</v>
       </c>
@@ -959,7 +960,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>43843</v>
       </c>
@@ -1000,7 +1001,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>43843</v>
       </c>
@@ -1041,7 +1042,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>43844</v>
       </c>
@@ -1082,7 +1083,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>43844</v>
       </c>
@@ -1123,7 +1124,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>43852</v>
       </c>
@@ -1164,7 +1165,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>43852</v>
       </c>
@@ -1205,7 +1206,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>43852</v>
       </c>
@@ -1246,7 +1247,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>43852</v>
       </c>
@@ -1287,7 +1288,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>43854</v>
       </c>
@@ -1328,7 +1329,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>43854</v>
       </c>
@@ -1369,7 +1370,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>43854</v>
       </c>
@@ -1410,7 +1411,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1425,7 +1426,7 @@
       <c r="L18" s="5"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1440,7 +1441,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1455,7 +1456,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1469,7 +1470,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1483,7 +1484,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1497,7 +1498,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1511,7 +1512,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1525,7 +1526,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1539,7 +1540,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1553,7 +1554,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1567,7 +1568,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1581,7 +1582,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1595,7 +1596,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1609,7 +1610,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1623,7 +1624,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1637,7 +1638,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1651,7 +1652,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1665,7 +1666,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1679,7 +1680,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1693,7 +1694,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1707,7 +1708,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1721,7 +1722,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1735,7 +1736,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1749,7 +1750,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1763,7 +1764,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1777,7 +1778,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1791,7 +1792,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1805,7 +1806,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1819,7 +1820,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1833,7 +1834,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1847,7 +1848,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1861,7 +1862,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1875,7 +1876,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1889,7 +1890,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1903,7 +1904,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1917,7 +1918,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1931,7 +1932,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1945,7 +1946,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1959,7 +1960,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1973,7 +1974,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1987,7 +1988,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2001,7 +2002,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2015,7 +2016,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2029,7 +2030,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2043,7 +2044,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2057,7 +2058,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2071,7 +2072,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2085,7 +2086,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2099,7 +2100,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2113,7 +2114,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2127,7 +2128,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2141,7 +2142,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2155,7 +2156,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2169,7 +2170,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2183,7 +2184,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2197,7 +2198,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2211,7 +2212,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2225,7 +2226,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2239,7 +2240,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2253,7 +2254,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2267,7 +2268,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2281,7 +2282,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2295,7 +2296,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2309,7 +2310,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2323,7 +2324,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2337,7 +2338,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2351,7 +2352,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2365,7 +2366,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2379,7 +2380,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2393,7 +2394,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2407,7 +2408,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2421,7 +2422,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2435,7 +2436,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2449,7 +2450,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2463,7 +2464,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2477,7 +2478,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2491,7 +2492,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2505,7 +2506,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2519,7 +2520,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2533,7 +2534,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2547,7 +2548,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2561,7 +2562,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2575,7 +2576,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2589,7 +2590,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2603,7 +2604,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2617,7 +2618,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2631,7 +2632,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2645,7 +2646,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2659,7 +2660,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2673,7 +2674,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2687,7 +2688,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2701,7 +2702,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2715,7 +2716,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2729,7 +2730,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2743,7 +2744,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -2757,7 +2758,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2771,7 +2772,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -2785,7 +2786,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2799,7 +2800,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -2813,7 +2814,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -2827,7 +2828,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -2841,7 +2842,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -2857,42 +2858,42 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E6" r:id="rId2"/>
-    <hyperlink ref="E7:E8" r:id="rId3" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-13-2020\"/>
-    <hyperlink ref="E9" r:id="rId4"/>
-    <hyperlink ref="E10" r:id="rId5"/>
-    <hyperlink ref="E11" r:id="rId6"/>
-    <hyperlink ref="E12:E14" r:id="rId7" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\"/>
-    <hyperlink ref="E16" r:id="rId8"/>
-    <hyperlink ref="E15" r:id="rId9"/>
-    <hyperlink ref="E17" r:id="rId10"/>
-    <hyperlink ref="E3" r:id="rId11"/>
-    <hyperlink ref="E4" r:id="rId12"/>
-    <hyperlink ref="E5" r:id="rId13"/>
-    <hyperlink ref="E7" r:id="rId14"/>
-    <hyperlink ref="E8" r:id="rId15"/>
-    <hyperlink ref="E12" r:id="rId16"/>
-    <hyperlink ref="E13" r:id="rId17"/>
-    <hyperlink ref="E14" r:id="rId18"/>
-    <hyperlink ref="L2" r:id="rId19"/>
-    <hyperlink ref="L3" r:id="rId20"/>
-    <hyperlink ref="L6" r:id="rId21"/>
-    <hyperlink ref="L9" r:id="rId22"/>
-    <hyperlink ref="L14" r:id="rId23"/>
-    <hyperlink ref="L17" r:id="rId24"/>
-    <hyperlink ref="L13" r:id="rId25"/>
-    <hyperlink ref="L4" r:id="rId26"/>
-    <hyperlink ref="L5" r:id="rId27"/>
-    <hyperlink ref="L7" r:id="rId28"/>
-    <hyperlink ref="L8" r:id="rId29"/>
-    <hyperlink ref="L10" r:id="rId30"/>
-    <hyperlink ref="L11:L12" r:id="rId31" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg"/>
-    <hyperlink ref="L11" r:id="rId32"/>
-    <hyperlink ref="L12" r:id="rId33"/>
-    <hyperlink ref="L15:L16" r:id="rId34" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg"/>
-    <hyperlink ref="L15" r:id="rId35"/>
-    <hyperlink ref="L16" r:id="rId36"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E7:E8" r:id="rId3" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-13-2020\" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E12:E14" r:id="rId7" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E16" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E15" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E3" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E4" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E5" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E7" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E8" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E12" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="L2" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="L3" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="L6" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="L9" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="L14" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="L17" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="L13" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="L4" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="L5" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="L7" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="L8" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="L10" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L11:L12" r:id="rId31" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="L11" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="L12" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="L15:L16" r:id="rId34" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="L15" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="L16" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>